<commit_message>
DOCS: READMD 초안 작성
</commit_message>
<xml_diff>
--- a/Backend/data/기업정보.xlsx
+++ b/Backend/data/기업정보.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\S05P21A302\Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF11F70-DC5B-4938-AE13-F769D81E006E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E4B961-FA7B-4462-8EEE-6D05F1BA4AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -655,9 +655,6 @@
     <t>셀트리온</t>
   </si>
   <si>
-    <t>기아</t>
-  </si>
-  <si>
     <t>현대모비스</t>
   </si>
   <si>
@@ -686,9 +683,6 @@
   </si>
   <si>
     <t>한국전력</t>
-  </si>
-  <si>
-    <t>LG</t>
   </si>
   <si>
     <t>삼성생명</t>
@@ -1823,10 +1817,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>대상㈜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>KB금융 KB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1836,6 +1826,18 @@
   </si>
   <si>
     <t>아모레퍼시픽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기아차</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상그룹</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2247,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="C198" sqref="C198"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="F196" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2278,7 +2280,7 @@
         <v>203</v>
       </c>
       <c r="D2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2292,7 +2294,7 @@
         <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2303,10 +2305,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2320,7 +2322,7 @@
         <v>205</v>
       </c>
       <c r="D5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2334,7 +2336,7 @@
         <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2348,7 +2350,7 @@
         <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2362,7 +2364,7 @@
         <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2376,7 +2378,7 @@
         <v>209</v>
       </c>
       <c r="D9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2390,7 +2392,7 @@
         <v>210</v>
       </c>
       <c r="D10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2401,10 +2403,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>600</v>
       </c>
       <c r="D11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2415,10 +2417,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2429,10 +2431,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2443,10 +2445,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2457,10 +2459,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2471,10 +2473,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2485,10 +2487,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D17" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2499,10 +2501,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2513,10 +2515,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2527,10 +2529,10 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D20" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2541,10 +2543,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2555,10 +2557,10 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2569,10 +2571,10 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2583,10 +2585,10 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2597,10 +2599,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>222</v>
+        <v>601</v>
       </c>
       <c r="D25" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2611,10 +2613,10 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D26" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2625,10 +2627,10 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2639,10 +2641,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2653,10 +2655,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D29" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2667,10 +2669,10 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2681,10 +2683,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D31" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2695,10 +2697,10 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D32" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2709,10 +2711,10 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D33" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2723,10 +2725,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D34" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2737,10 +2739,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D35" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2751,10 +2753,10 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D36" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2765,10 +2767,10 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D37" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2779,10 +2781,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2793,10 +2795,10 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D39" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2807,10 +2809,10 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D40" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2821,10 +2823,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D41" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2835,10 +2837,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D42" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2849,10 +2851,10 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D43" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2863,10 +2865,10 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D44" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2877,10 +2879,10 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D45" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2891,10 +2893,10 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D46" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2905,10 +2907,10 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D47" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2919,10 +2921,10 @@
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D48" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2933,10 +2935,10 @@
         <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D49" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2947,10 +2949,10 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D50" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2961,10 +2963,10 @@
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D51" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2975,10 +2977,10 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D52" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2989,10 +2991,10 @@
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D53" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -3003,10 +3005,10 @@
         <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D54" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3017,10 +3019,10 @@
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D55" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -3031,10 +3033,10 @@
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D56" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -3045,10 +3047,10 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D57" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -3059,10 +3061,10 @@
         <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D58" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -3073,10 +3075,10 @@
         <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D59" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -3087,10 +3089,10 @@
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D60" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -3101,10 +3103,10 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D61" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -3115,10 +3117,10 @@
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -3129,10 +3131,10 @@
         <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D63" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -3143,10 +3145,10 @@
         <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D64" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3157,10 +3159,10 @@
         <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D65" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -3171,10 +3173,10 @@
         <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D66" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3185,10 +3187,10 @@
         <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D67" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3199,10 +3201,10 @@
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D68" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3213,10 +3215,10 @@
         <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D69" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3227,10 +3229,10 @@
         <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D70" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3241,10 +3243,10 @@
         <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3255,10 +3257,10 @@
         <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D72" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3269,10 +3271,10 @@
         <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D73" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3283,10 +3285,10 @@
         <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D74" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -3297,10 +3299,10 @@
         <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D75" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3311,10 +3313,10 @@
         <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D76" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -3325,10 +3327,10 @@
         <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D77" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3339,10 +3341,10 @@
         <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D78" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -3353,10 +3355,10 @@
         <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D79" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3367,10 +3369,10 @@
         <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D80" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3381,10 +3383,10 @@
         <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D81" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -3395,10 +3397,10 @@
         <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D82" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -3409,10 +3411,10 @@
         <v>84</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D83" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -3423,10 +3425,10 @@
         <v>85</v>
       </c>
       <c r="C84" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D84" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -3437,10 +3439,10 @@
         <v>86</v>
       </c>
       <c r="C85" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D85" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3451,10 +3453,10 @@
         <v>87</v>
       </c>
       <c r="C86" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D86" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -3465,10 +3467,10 @@
         <v>88</v>
       </c>
       <c r="C87" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D87" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -3479,10 +3481,10 @@
         <v>89</v>
       </c>
       <c r="C88" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D88" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3493,10 +3495,10 @@
         <v>90</v>
       </c>
       <c r="C89" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D89" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3507,10 +3509,10 @@
         <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D90" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -3521,10 +3523,10 @@
         <v>92</v>
       </c>
       <c r="C91" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D91" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -3535,10 +3537,10 @@
         <v>93</v>
       </c>
       <c r="C92" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D92" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -3549,10 +3551,10 @@
         <v>94</v>
       </c>
       <c r="C93" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D93" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -3563,10 +3565,10 @@
         <v>95</v>
       </c>
       <c r="C94" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D94" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -3577,10 +3579,10 @@
         <v>96</v>
       </c>
       <c r="C95" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D95" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -3591,10 +3593,10 @@
         <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D96" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3605,10 +3607,10 @@
         <v>98</v>
       </c>
       <c r="C97" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D97" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3619,10 +3621,10 @@
         <v>99</v>
       </c>
       <c r="C98" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D98" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3633,10 +3635,10 @@
         <v>100</v>
       </c>
       <c r="C99" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D99" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -3647,10 +3649,10 @@
         <v>101</v>
       </c>
       <c r="C100" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D100" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -3661,10 +3663,10 @@
         <v>102</v>
       </c>
       <c r="C101" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D101" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -3675,10 +3677,10 @@
         <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D102" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -3689,10 +3691,10 @@
         <v>104</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D103" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -3703,10 +3705,10 @@
         <v>105</v>
       </c>
       <c r="C104" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D104" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -3717,10 +3719,10 @@
         <v>106</v>
       </c>
       <c r="C105" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D105" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -3731,10 +3733,10 @@
         <v>107</v>
       </c>
       <c r="C106" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D106" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3745,10 +3747,10 @@
         <v>108</v>
       </c>
       <c r="C107" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D107" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3759,10 +3761,10 @@
         <v>109</v>
       </c>
       <c r="C108" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D108" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3773,10 +3775,10 @@
         <v>110</v>
       </c>
       <c r="C109" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D109" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3787,10 +3789,10 @@
         <v>111</v>
       </c>
       <c r="C110" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D110" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -3801,10 +3803,10 @@
         <v>112</v>
       </c>
       <c r="C111" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D111" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -3815,10 +3817,10 @@
         <v>113</v>
       </c>
       <c r="C112" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D112" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -3829,10 +3831,10 @@
         <v>114</v>
       </c>
       <c r="C113" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D113" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3843,10 +3845,10 @@
         <v>115</v>
       </c>
       <c r="C114" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D114" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -3857,10 +3859,10 @@
         <v>116</v>
       </c>
       <c r="C115" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D115" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -3871,10 +3873,10 @@
         <v>117</v>
       </c>
       <c r="C116" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D116" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3885,10 +3887,10 @@
         <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D117" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -3899,10 +3901,10 @@
         <v>119</v>
       </c>
       <c r="C118" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D118" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -3913,10 +3915,10 @@
         <v>120</v>
       </c>
       <c r="C119" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D119" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -3927,10 +3929,10 @@
         <v>121</v>
       </c>
       <c r="C120" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D120" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -3941,10 +3943,10 @@
         <v>122</v>
       </c>
       <c r="C121" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D121" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -3955,10 +3957,10 @@
         <v>123</v>
       </c>
       <c r="C122" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D122" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -3969,10 +3971,10 @@
         <v>124</v>
       </c>
       <c r="C123" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D123" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -3983,10 +3985,10 @@
         <v>125</v>
       </c>
       <c r="C124" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D124" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -3997,10 +3999,10 @@
         <v>126</v>
       </c>
       <c r="C125" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D125" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -4011,10 +4013,10 @@
         <v>127</v>
       </c>
       <c r="C126" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D126" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -4025,10 +4027,10 @@
         <v>128</v>
       </c>
       <c r="C127" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D127" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -4039,10 +4041,10 @@
         <v>129</v>
       </c>
       <c r="C128" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D128" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -4053,10 +4055,10 @@
         <v>130</v>
       </c>
       <c r="C129" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D129" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -4067,10 +4069,10 @@
         <v>131</v>
       </c>
       <c r="C130" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D130" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -4081,10 +4083,10 @@
         <v>132</v>
       </c>
       <c r="C131" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D131" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -4095,10 +4097,10 @@
         <v>133</v>
       </c>
       <c r="C132" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D132" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -4109,10 +4111,10 @@
         <v>134</v>
       </c>
       <c r="C133" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D133" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -4123,10 +4125,10 @@
         <v>135</v>
       </c>
       <c r="C134" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D134" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -4137,10 +4139,10 @@
         <v>136</v>
       </c>
       <c r="C135" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D135" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -4151,10 +4153,10 @@
         <v>137</v>
       </c>
       <c r="C136" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D136" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -4165,10 +4167,10 @@
         <v>138</v>
       </c>
       <c r="C137" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D137" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -4179,10 +4181,10 @@
         <v>139</v>
       </c>
       <c r="C138" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D138" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -4193,10 +4195,10 @@
         <v>140</v>
       </c>
       <c r="C139" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -4207,10 +4209,10 @@
         <v>141</v>
       </c>
       <c r="C140" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D140" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -4221,10 +4223,10 @@
         <v>142</v>
       </c>
       <c r="C141" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D141" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -4235,10 +4237,10 @@
         <v>143</v>
       </c>
       <c r="C142" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D142" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -4249,10 +4251,10 @@
         <v>144</v>
       </c>
       <c r="C143" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D143" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -4263,10 +4265,10 @@
         <v>145</v>
       </c>
       <c r="C144" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D144" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -4277,10 +4279,10 @@
         <v>146</v>
       </c>
       <c r="C145" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D145" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -4291,10 +4293,10 @@
         <v>147</v>
       </c>
       <c r="C146" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D146" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -4305,10 +4307,10 @@
         <v>148</v>
       </c>
       <c r="C147" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D147" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -4319,10 +4321,10 @@
         <v>149</v>
       </c>
       <c r="C148" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D148" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -4333,10 +4335,10 @@
         <v>150</v>
       </c>
       <c r="C149" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D149" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -4347,10 +4349,10 @@
         <v>151</v>
       </c>
       <c r="C150" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D150" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -4361,10 +4363,10 @@
         <v>152</v>
       </c>
       <c r="C151" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D151" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -4375,10 +4377,10 @@
         <v>153</v>
       </c>
       <c r="C152" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D152" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -4389,10 +4391,10 @@
         <v>154</v>
       </c>
       <c r="C153" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D153" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -4403,10 +4405,10 @@
         <v>155</v>
       </c>
       <c r="C154" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D154" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -4417,10 +4419,10 @@
         <v>156</v>
       </c>
       <c r="C155" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D155" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -4431,10 +4433,10 @@
         <v>157</v>
       </c>
       <c r="C156" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D156" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -4445,10 +4447,10 @@
         <v>158</v>
       </c>
       <c r="C157" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D157" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -4459,10 +4461,10 @@
         <v>159</v>
       </c>
       <c r="C158" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D158" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -4473,10 +4475,10 @@
         <v>160</v>
       </c>
       <c r="C159" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D159" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -4487,10 +4489,10 @@
         <v>161</v>
       </c>
       <c r="C160" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D160" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -4501,10 +4503,10 @@
         <v>162</v>
       </c>
       <c r="C161" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D161" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -4515,10 +4517,10 @@
         <v>163</v>
       </c>
       <c r="C162" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D162" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -4529,10 +4531,10 @@
         <v>164</v>
       </c>
       <c r="C163" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D163" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -4543,10 +4545,10 @@
         <v>165</v>
       </c>
       <c r="C164" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D164" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -4557,10 +4559,10 @@
         <v>166</v>
       </c>
       <c r="C165" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D165" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
@@ -4571,10 +4573,10 @@
         <v>167</v>
       </c>
       <c r="C166" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D166" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -4585,10 +4587,10 @@
         <v>168</v>
       </c>
       <c r="C167" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D167" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -4599,10 +4601,10 @@
         <v>169</v>
       </c>
       <c r="C168" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D168" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -4613,10 +4615,10 @@
         <v>170</v>
       </c>
       <c r="C169" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D169" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -4627,10 +4629,10 @@
         <v>171</v>
       </c>
       <c r="C170" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D170" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -4641,10 +4643,10 @@
         <v>172</v>
       </c>
       <c r="C171" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D171" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -4655,10 +4657,10 @@
         <v>173</v>
       </c>
       <c r="C172" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D172" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -4669,10 +4671,10 @@
         <v>174</v>
       </c>
       <c r="C173" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D173" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -4683,10 +4685,10 @@
         <v>175</v>
       </c>
       <c r="C174" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D174" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -4697,10 +4699,10 @@
         <v>176</v>
       </c>
       <c r="C175" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D175" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -4711,10 +4713,10 @@
         <v>177</v>
       </c>
       <c r="C176" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D176" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -4725,10 +4727,10 @@
         <v>178</v>
       </c>
       <c r="C177" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D177" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -4739,10 +4741,10 @@
         <v>179</v>
       </c>
       <c r="C178" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D178" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -4753,10 +4755,10 @@
         <v>180</v>
       </c>
       <c r="C179" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D179" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -4767,10 +4769,10 @@
         <v>181</v>
       </c>
       <c r="C180" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D180" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -4781,10 +4783,10 @@
         <v>182</v>
       </c>
       <c r="C181" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D181" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -4795,10 +4797,10 @@
         <v>183</v>
       </c>
       <c r="C182" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D182" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -4809,10 +4811,10 @@
         <v>184</v>
       </c>
       <c r="C183" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D183" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -4823,10 +4825,10 @@
         <v>185</v>
       </c>
       <c r="C184" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D184" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -4837,10 +4839,10 @@
         <v>186</v>
       </c>
       <c r="C185" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D185" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -4851,10 +4853,10 @@
         <v>187</v>
       </c>
       <c r="C186" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D186" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -4865,10 +4867,10 @@
         <v>188</v>
       </c>
       <c r="C187" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D187" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -4879,10 +4881,10 @@
         <v>189</v>
       </c>
       <c r="C188" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D188" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -4893,10 +4895,10 @@
         <v>190</v>
       </c>
       <c r="C189" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D189" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -4907,10 +4909,10 @@
         <v>191</v>
       </c>
       <c r="C190" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D190" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -4921,10 +4923,10 @@
         <v>192</v>
       </c>
       <c r="C191" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D191" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
@@ -4935,10 +4937,10 @@
         <v>193</v>
       </c>
       <c r="C192" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D192" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
@@ -4949,10 +4951,10 @@
         <v>194</v>
       </c>
       <c r="C193" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D193" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
@@ -4963,10 +4965,10 @@
         <v>195</v>
       </c>
       <c r="C194" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D194" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
@@ -4977,10 +4979,10 @@
         <v>196</v>
       </c>
       <c r="C195" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D195" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
@@ -4991,10 +4993,10 @@
         <v>197</v>
       </c>
       <c r="C196" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D196" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
@@ -5005,10 +5007,10 @@
         <v>198</v>
       </c>
       <c r="C197" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D197" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
@@ -5019,10 +5021,10 @@
         <v>199</v>
       </c>
       <c r="C198" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D198" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
@@ -5033,10 +5035,10 @@
         <v>200</v>
       </c>
       <c r="C199" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D199" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
@@ -5047,10 +5049,10 @@
         <v>201</v>
       </c>
       <c r="C200" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D200" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
@@ -5061,10 +5063,10 @@
         <v>202</v>
       </c>
       <c r="C201" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D201" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>